<commit_message>
Fix firefox tests, fix test cases and bugs report
</commit_message>
<xml_diff>
--- a/TestCases&Bugs.xlsx
+++ b/TestCases&Bugs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Test Case #</t>
   </si>
@@ -46,37 +46,19 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Dialog appears after clicking the perimeter</t>
-  </si>
-  <si>
-    <t>After last icon is clicked, a dialog message appears asking for a next size</t>
-  </si>
-  <si>
     <t>"-"</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>Click the outer icons in the grid of "Your playground"</t>
-  </si>
-  <si>
-    <t>Dialog does not appear when clicking the icons in the grid</t>
-  </si>
-  <si>
     <t>Grid has rows and columns of the number specified in the dialog</t>
   </si>
   <si>
-    <t>A prompt is shown explaining that the number is incorrect</t>
-  </si>
-  <si>
     <t>Prompt shows "Not a good size!"</t>
   </si>
   <si>
     <t>Enter strings in the dialog</t>
-  </si>
-  <si>
-    <t>Outer perimeter is clicked on url "https://keenonred.github.io"</t>
   </si>
   <si>
     <t>url "https://keenonred.github.io" is open</t>
@@ -100,14 +82,6 @@
     <t>Enter valid width and height in the url</t>
   </si>
   <si>
-    <t>1. To the url add /?width=5&amp;height=4
-2. Press enter
-3. Repeat with width = 8, height = 9</t>
-  </si>
-  <si>
-    <t>Grid changes to 5 columns and 4 rows and 8 columns and 9 rows, respectively</t>
-  </si>
-  <si>
     <t>Enter invalid width and height in the url</t>
   </si>
   <si>
@@ -158,12 +132,6 @@
 3. Repeat with number "10"</t>
   </si>
   <si>
-    <t>Dialog does not appear when more than perimeter icons are marked</t>
-  </si>
-  <si>
-    <t>Mark all more items than the perimeter</t>
-  </si>
-  <si>
     <t>Grid defaults to 4x4 as it should not accept a width of 2</t>
   </si>
   <si>
@@ -241,16 +209,52 @@
   <si>
     <t>1. Open url "https://keenonred.github.io"
 2. Press just on the right side of the icon</t>
+  </si>
+  <si>
+    <t>Dialog appears after clicking the perimeter icons</t>
+  </si>
+  <si>
+    <t>Click the perimeter icons in the grid of "Your playground"</t>
+  </si>
+  <si>
+    <t>After the last icon is clicked, a dialog message appears asking for the next size</t>
+  </si>
+  <si>
+    <t>Dialog does not appear when more than just the perimeter icons are marked</t>
+  </si>
+  <si>
+    <t>1. Click at least one non-perimeter icon
+2. Click all the perimeter icons</t>
+  </si>
+  <si>
+    <t>Perimeter icons are clicked on url "https://keenonred.github.io"</t>
+  </si>
+  <si>
+    <t>A prompt is shown explaining that the number is incorrect and the grid defaults to 4x4</t>
+  </si>
+  <si>
+    <t>1. At the end of the url add /?width=5&amp;height=4
+2. Press enter
+3. Repeat with width = 8, height = 9</t>
+  </si>
+  <si>
+    <t>Grid changes to 5 columns and 4 rows / 8 columns and 9 rows, respectively</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -276,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -305,31 +309,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -350,36 +387,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,18 +445,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:J11" totalsRowShown="0" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:J11" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="B2:J11"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Test Case #" dataDxfId="17"/>
-    <tableColumn id="2" name="Description" dataDxfId="16"/>
-    <tableColumn id="3" name="Precondition" dataDxfId="15"/>
-    <tableColumn id="4" name="Steps" dataDxfId="14"/>
-    <tableColumn id="5" name="Expected Result" dataDxfId="13"/>
-    <tableColumn id="6" name="Actual Result" dataDxfId="12"/>
-    <tableColumn id="7" name="Status" dataDxfId="11"/>
-    <tableColumn id="9" name="Bug #" dataDxfId="9"/>
-    <tableColumn id="8" name="Notes" dataDxfId="10"/>
+    <tableColumn id="1" name="Test Case #" dataDxfId="15"/>
+    <tableColumn id="2" name="Description" dataDxfId="14"/>
+    <tableColumn id="3" name="Precondition" dataDxfId="13"/>
+    <tableColumn id="4" name="Steps" dataDxfId="12"/>
+    <tableColumn id="5" name="Expected Result" dataDxfId="11"/>
+    <tableColumn id="6" name="Actual Result" dataDxfId="10"/>
+    <tableColumn id="7" name="Status" dataDxfId="9"/>
+    <tableColumn id="9" name="Bug #" dataDxfId="8"/>
+    <tableColumn id="8" name="Notes" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -459,13 +466,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:H7" totalsRowShown="0">
   <autoFilter ref="B2:H7"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Bug #" dataDxfId="0"/>
-    <tableColumn id="2" name="Description" dataDxfId="1"/>
-    <tableColumn id="3" name="Reproduction steps" dataDxfId="6"/>
-    <tableColumn id="6" name="Expected Result" dataDxfId="5"/>
-    <tableColumn id="7" name="Actual Result" dataDxfId="4"/>
-    <tableColumn id="4" name="Priority (1 high-5 low)" dataDxfId="3"/>
-    <tableColumn id="5" name="Severity (1 high -5 low)" dataDxfId="2"/>
+    <tableColumn id="1" name="Bug #" dataDxfId="6"/>
+    <tableColumn id="2" name="Description" dataDxfId="5"/>
+    <tableColumn id="3" name="Reproduction steps" dataDxfId="4"/>
+    <tableColumn id="6" name="Expected Result" dataDxfId="3"/>
+    <tableColumn id="7" name="Actual Result" dataDxfId="2"/>
+    <tableColumn id="4" name="Priority (1 high-5 low)" dataDxfId="1"/>
+    <tableColumn id="5" name="Severity (1 high -5 low)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +785,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>7</v>
@@ -789,46 +796,46 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="2:10" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
+      <c r="C4" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>
@@ -838,22 +845,22 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
@@ -863,22 +870,22 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
@@ -888,22 +895,22 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
@@ -915,22 +922,22 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="2"/>
@@ -940,22 +947,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I9" s="3">
         <v>2</v>
@@ -967,28 +974,28 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I10" s="3">
         <v>3</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -996,42 +1003,43 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I11" s="3">
         <v>4</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H3:H11">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1056,13 +1064,13 @@
   <sheetData>
     <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1071,10 +1079,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="105" x14ac:dyDescent="0.25">
@@ -1082,16 +1090,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G3" s="9">
         <v>4</v>
@@ -1105,16 +1113,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G4" s="9">
         <v>2</v>
@@ -1128,16 +1136,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G5" s="9">
         <v>3</v>
@@ -1151,16 +1159,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G6" s="9">
         <v>1</v>
@@ -1174,16 +1182,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G7" s="9">
         <v>5</v>

</xml_diff>